<commit_message>
Fixes to Project 4
</commit_message>
<xml_diff>
--- a/performance_results.xlsx
+++ b/performance_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Documents\GitHub\ACS-Project-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FBECF782-03F0-4CD3-B2BE-F1E8DE9AE83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{873C7847-0188-4318-8051-86202D19FBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{02613F9A-C2E5-4855-833B-E06CE7E89CE8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1BAA38E5-83EE-4B4D-8087-797CE21B9F03}"/>
   </bookViews>
   <sheets>
     <sheet name="performance_results" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
-    <t>Operation</t>
+    <t>TestType</t>
   </si>
   <si>
-    <t>Threads</t>
+    <t>Users/Threads</t>
   </si>
   <si>
     <t>Time(s)</t>
   </si>
   <si>
-    <t>Encoding</t>
+    <t>Extra</t>
   </si>
   <si>
-    <t>Query</t>
+    <t>EncodingPerformance</t>
+  </si>
+  <si>
+    <t>VanillaColumnScan</t>
+  </si>
+  <si>
+    <t>QuerySingleItem</t>
+  </si>
+  <si>
+    <t>Non-SIMD</t>
+  </si>
+  <si>
+    <t>SIMD</t>
+  </si>
+  <si>
+    <t>VanillaPrefixScan</t>
+  </si>
+  <si>
+    <t>QueryPrefixScan</t>
+  </si>
+  <si>
+    <t>ValueSizeTest</t>
+  </si>
+  <si>
+    <t>8 bytes</t>
+  </si>
+  <si>
+    <t>64 bytes</t>
+  </si>
+  <si>
+    <t>256 bytes</t>
+  </si>
+  <si>
+    <t>4 bytes</t>
+  </si>
+  <si>
+    <t>16 bytes</t>
+  </si>
+  <si>
+    <t>32 bytes</t>
+  </si>
+  <si>
+    <t>128 bytes</t>
   </si>
 </sst>
 </file>
@@ -518,12 +560,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -616,12 +655,15 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Encoding Time vs</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>. Number of Threads</a:t>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Encoding Time vs. Number of Threads</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -664,17 +706,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>performance_results!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Time(s)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -763,52 +794,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>8.9330300000000001E-2</c:v>
+                  <c:v>9.7296599999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8576200000000004E-2</c:v>
+                  <c:v>7.2206900000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.1198799999999998E-2</c:v>
+                  <c:v>6.9512199999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.24351E-2</c:v>
+                  <c:v>6.8735299999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8288800000000002E-2</c:v>
+                  <c:v>6.6747399999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.8939100000000001E-2</c:v>
+                  <c:v>7.1371400000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.90882E-2</c:v>
+                  <c:v>6.8592799999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.6203100000000001E-2</c:v>
+                  <c:v>6.0753700000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.5832500000000002E-2</c:v>
+                  <c:v>6.0248599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0273E-2</c:v>
+                  <c:v>5.5409300000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.6103300000000002E-2</c:v>
+                  <c:v>5.6318E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.2645000000000006E-2</c:v>
+                  <c:v>6.33407E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.31776E-2</c:v>
+                  <c:v>5.4628799999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.2632699999999999E-2</c:v>
+                  <c:v>5.7823899999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.8807999999999994E-2</c:v>
+                  <c:v>6.2732599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.2276199999999997E-2</c:v>
+                  <c:v>6.3052200000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -816,7 +847,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-076D-4D03-9367-6EB7107CC0CF}"/>
+              <c16:uniqueId val="{00000000-676A-45C4-8235-A4C6FA829A3D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -828,11 +859,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80118496"/>
-        <c:axId val="80118016"/>
+        <c:axId val="1441051840"/>
+        <c:axId val="1441048960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80118496"/>
+        <c:axId val="1441051840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="16"/>
@@ -874,7 +905,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Number of Threads</a:t>
                 </a:r>
               </a:p>
@@ -946,14 +984,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80118016"/>
+        <c:crossAx val="1441048960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80118016"/>
+        <c:axId val="1441048960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
           <c:min val="5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -992,14 +1033,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Time</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Time  (s)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t>  (s)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1069,7 +1112,482 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80118496"/>
+        <c:crossAx val="1441051840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Encoding</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Time vs. Value Size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>performance_results!$B$24:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>performance_results!$C$24:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.9138699999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3560899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3920900000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9347099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6354899999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11988</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15062800000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3C20-4B12-A30F-E1ECBDD4B6A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1522848448"/>
+        <c:axId val="1522852768"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1522848448"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Value Size (Bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1522852768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1522852768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.16000000000000003"/>
+          <c:min val="6.0000000000000012E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1522848448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1165,6 +1683,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1681,19 +2239,535 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1701,7 +2775,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ECF814E-CAF3-AB71-2542-302D655F9388}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{630E30AF-3384-2E54-AD23-C89B6AE053EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1714,6 +2788,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D84E2F32-A4D4-C68A-5577-29391B93AF3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2038,17 +3148,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CDAE79-2995-4AED-90EB-DFAC723E30DB}">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB150BC-B959-470D-9EDB-FC4AC450BEA7}">
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2057,192 +3167,360 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>8.9330300000000001E-2</v>
+        <v>9.7296599999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>6.8576200000000004E-2</v>
+        <v>7.2206900000000004E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>6.1198799999999998E-2</v>
+        <v>6.9512199999999996E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>6.24351E-2</v>
+        <v>6.8735299999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>5.8288800000000002E-2</v>
+        <v>6.6747399999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>5.8939100000000001E-2</v>
+        <v>7.1371400000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>5.90882E-2</v>
+        <v>6.8592799999999995E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>6.6203100000000001E-2</v>
+        <v>6.0753700000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>6.5832500000000002E-2</v>
+        <v>6.0248599999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>6.0273E-2</v>
+        <v>5.5409300000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>5.6103300000000002E-2</v>
+        <v>5.6318E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>6.2645000000000006E-2</v>
+        <v>6.33407E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>6.31776E-2</v>
+        <v>5.4628799999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>6.2632699999999999E-2</v>
+        <v>5.7823899999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>6.8807999999999994E-2</v>
+        <v>6.2732599999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>6.2276199999999997E-2</v>
+        <v>6.3052200000000003E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
-        <v>1.8649999999999999E-6</v>
+      <c r="C18">
+        <v>8.6685699999999996E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3.9553899999999998E-4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2.9632E-5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1.0939999999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1.23783E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>8.1546900000000005E-2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>6.9138699999999997E-2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>7.3560899999999999E-2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26">
+        <v>9.3920900000000002E-2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <v>8.9347099999999999E-2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>9.6354899999999993E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>128</v>
+      </c>
+      <c r="C29">
+        <v>0.11988</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>256</v>
+      </c>
+      <c r="C30">
+        <v>0.15062800000000001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>